<commit_message>
Updated AnchorHeights to have error for all 5 tag positions and the average error.
</commit_message>
<xml_diff>
--- a/AnchorHeights.xlsx
+++ b/AnchorHeights.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>A</t>
   </si>
@@ -76,6 +76,87 @@
   </si>
   <si>
     <t>ActualZ_5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ActualX_1</t>
+  </si>
+  <si>
+    <t>ActualY_1</t>
+  </si>
+  <si>
+    <t>ActualZ_1</t>
+  </si>
+  <si>
+    <t>ActualX_2</t>
+  </si>
+  <si>
+    <t>ActualY_2</t>
+  </si>
+  <si>
+    <t>ActualZ_2</t>
+  </si>
+  <si>
+    <t>ActualX_3</t>
+  </si>
+  <si>
+    <t>ActualY_3</t>
+  </si>
+  <si>
+    <t>ActualZ_3</t>
+  </si>
+  <si>
+    <t>ActualX_4</t>
+  </si>
+  <si>
+    <t>ActualY_4</t>
+  </si>
+  <si>
+    <t>ActualZ_4</t>
+  </si>
+  <si>
+    <t>ActualX_5</t>
+  </si>
+  <si>
+    <t>ActualY_5</t>
+  </si>
+  <si>
+    <t>ActualZ_5</t>
+  </si>
+  <si>
+    <t>Error1</t>
+  </si>
+  <si>
+    <t>Error2</t>
+  </si>
+  <si>
+    <t>Error3</t>
+  </si>
+  <si>
+    <t>Error4</t>
+  </si>
+  <si>
+    <t>Error5</t>
+  </si>
+  <si>
+    <t>ErrorAverage</t>
   </si>
 </sst>
 </file>
@@ -121,7 +202,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:AA26"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="true"/>
@@ -145,91 +226,115 @@
     <col min="19" max="19" width="9.85546875" customWidth="true"/>
     <col min="20" max="20" width="9.7109375" customWidth="true"/>
     <col min="21" max="21" width="9.7109375" customWidth="true"/>
+    <col min="22" max="22" width="6.42578125" customWidth="true"/>
+    <col min="23" max="23" width="6.42578125" customWidth="true"/>
+    <col min="24" max="24" width="6.42578125" customWidth="true"/>
+    <col min="25" max="25" width="6.42578125" customWidth="true"/>
+    <col min="26" max="26" width="6.42578125" customWidth="true"/>
+    <col min="27" max="27" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>20</v>
+        <v>41</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B2" s="0">
-        <v>6</v>
+        <v>195</v>
       </c>
       <c r="C2" s="0">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="D2" s="0">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="E2" s="0">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="F2" s="0">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G2" s="0">
         <v>0</v>
@@ -274,27 +379,45 @@
         <v>0</v>
       </c>
       <c r="U2" s="0">
+        <v>0</v>
+      </c>
+      <c r="V2" s="0">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0">
+        <v>0</v>
+      </c>
+      <c r="X2" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B3" s="0">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D3" s="0">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="E3" s="0">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="G3" s="0">
         <v>0</v>
@@ -339,27 +462,45 @@
         <v>0</v>
       </c>
       <c r="U3" s="0">
+        <v>0</v>
+      </c>
+      <c r="V3" s="0">
+        <v>0</v>
+      </c>
+      <c r="W3" s="0">
+        <v>0</v>
+      </c>
+      <c r="X3" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B4" s="0">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="C4" s="0">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="D4" s="0">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E4" s="0">
-        <v>161</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="G4" s="0">
         <v>0</v>
@@ -404,27 +545,45 @@
         <v>0</v>
       </c>
       <c r="U4" s="0">
+        <v>0</v>
+      </c>
+      <c r="V4" s="0">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0">
+        <v>0</v>
+      </c>
+      <c r="X4" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="B5" s="0">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C5" s="0">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="D5" s="0">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E5" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F5" s="0">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="G5" s="0">
         <v>0</v>
@@ -469,27 +628,45 @@
         <v>0</v>
       </c>
       <c r="U5" s="0">
+        <v>0</v>
+      </c>
+      <c r="V5" s="0">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0">
+        <v>0</v>
+      </c>
+      <c r="X5" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="B6" s="0">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="C6" s="0">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="D6" s="0">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="E6" s="0">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G6" s="0">
         <v>0</v>
@@ -534,27 +711,45 @@
         <v>0</v>
       </c>
       <c r="U6" s="0">
+        <v>0</v>
+      </c>
+      <c r="V6" s="0">
+        <v>0</v>
+      </c>
+      <c r="W6" s="0">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B7" s="0">
-        <v>177</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D7" s="0">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E7" s="0">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="F7" s="0">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="G7" s="0">
         <v>0</v>
@@ -599,27 +794,45 @@
         <v>0</v>
       </c>
       <c r="U7" s="0">
+        <v>0</v>
+      </c>
+      <c r="V7" s="0">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0">
+        <v>0</v>
+      </c>
+      <c r="X7" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B8" s="0">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="C8" s="0">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="D8" s="0">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="E8" s="0">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="F8" s="0">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="G8" s="0">
         <v>0</v>
@@ -664,27 +877,45 @@
         <v>0</v>
       </c>
       <c r="U8" s="0">
+        <v>0</v>
+      </c>
+      <c r="V8" s="0">
+        <v>0</v>
+      </c>
+      <c r="W8" s="0">
+        <v>0</v>
+      </c>
+      <c r="X8" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>32</v>
+        <v>190</v>
       </c>
       <c r="B9" s="0">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="C9" s="0">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="D9" s="0">
-        <v>155</v>
+        <v>47</v>
       </c>
       <c r="E9" s="0">
-        <v>159</v>
+        <v>26</v>
       </c>
       <c r="F9" s="0">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="G9" s="0">
         <v>0</v>
@@ -729,27 +960,45 @@
         <v>0</v>
       </c>
       <c r="U9" s="0">
+        <v>0</v>
+      </c>
+      <c r="V9" s="0">
+        <v>0</v>
+      </c>
+      <c r="W9" s="0">
+        <v>0</v>
+      </c>
+      <c r="X9" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="C10" s="0">
-        <v>3</v>
+        <v>195</v>
       </c>
       <c r="D10" s="0">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="E10" s="0">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="F10" s="0">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="G10" s="0">
         <v>0</v>
@@ -794,27 +1043,45 @@
         <v>0</v>
       </c>
       <c r="U10" s="0">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0">
+        <v>0</v>
+      </c>
+      <c r="X10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B11" s="0">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="C11" s="0">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="D11" s="0">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="E11" s="0">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="F11" s="0">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="G11" s="0">
         <v>0</v>
@@ -859,27 +1126,45 @@
         <v>0</v>
       </c>
       <c r="U11" s="0">
+        <v>0</v>
+      </c>
+      <c r="V11" s="0">
+        <v>0</v>
+      </c>
+      <c r="W11" s="0">
+        <v>0</v>
+      </c>
+      <c r="X11" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E12" s="0">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="F12" s="0">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="G12" s="0">
         <v>0</v>
@@ -924,27 +1209,45 @@
         <v>0</v>
       </c>
       <c r="U12" s="0">
+        <v>0</v>
+      </c>
+      <c r="V12" s="0">
+        <v>0</v>
+      </c>
+      <c r="W12" s="0">
+        <v>0</v>
+      </c>
+      <c r="X12" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="B13" s="0">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="C13" s="0">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D13" s="0">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E13" s="0">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="F13" s="0">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="G13" s="0">
         <v>0</v>
@@ -989,27 +1292,45 @@
         <v>0</v>
       </c>
       <c r="U13" s="0">
+        <v>0</v>
+      </c>
+      <c r="V13" s="0">
+        <v>0</v>
+      </c>
+      <c r="W13" s="0">
+        <v>0</v>
+      </c>
+      <c r="X13" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B14" s="0">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C14" s="0">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="D14" s="0">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="E14" s="0">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="F14" s="0">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="G14" s="0">
         <v>0</v>
@@ -1054,27 +1375,45 @@
         <v>0</v>
       </c>
       <c r="U14" s="0">
+        <v>0</v>
+      </c>
+      <c r="V14" s="0">
+        <v>0</v>
+      </c>
+      <c r="W14" s="0">
+        <v>0</v>
+      </c>
+      <c r="X14" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C15" s="0">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="D15" s="0">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="E15" s="0">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="F15" s="0">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="G15" s="0">
         <v>0</v>
@@ -1119,27 +1458,45 @@
         <v>0</v>
       </c>
       <c r="U15" s="0">
+        <v>0</v>
+      </c>
+      <c r="V15" s="0">
+        <v>0</v>
+      </c>
+      <c r="W15" s="0">
+        <v>0</v>
+      </c>
+      <c r="X15" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="B16" s="0">
-        <v>177</v>
+        <v>62</v>
       </c>
       <c r="C16" s="0">
-        <v>180</v>
+        <v>68</v>
       </c>
       <c r="D16" s="0">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="E16" s="0">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="F16" s="0">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="G16" s="0">
         <v>0</v>
@@ -1184,27 +1541,45 @@
         <v>0</v>
       </c>
       <c r="U16" s="0">
+        <v>0</v>
+      </c>
+      <c r="V16" s="0">
+        <v>0</v>
+      </c>
+      <c r="W16" s="0">
+        <v>0</v>
+      </c>
+      <c r="X16" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="0">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="C17" s="0">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="D17" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="0">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F17" s="0">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="G17" s="0">
         <v>0</v>
@@ -1249,27 +1624,45 @@
         <v>0</v>
       </c>
       <c r="U17" s="0">
+        <v>0</v>
+      </c>
+      <c r="V17" s="0">
+        <v>0</v>
+      </c>
+      <c r="W17" s="0">
+        <v>0</v>
+      </c>
+      <c r="X17" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C18" s="0">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="D18" s="0">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="E18" s="0">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="F18" s="0">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G18" s="0">
         <v>0</v>
@@ -1314,27 +1707,45 @@
         <v>0</v>
       </c>
       <c r="U18" s="0">
+        <v>0</v>
+      </c>
+      <c r="V18" s="0">
+        <v>0</v>
+      </c>
+      <c r="W18" s="0">
+        <v>0</v>
+      </c>
+      <c r="X18" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
+        <v>2</v>
+      </c>
+      <c r="B19" s="0">
         <v>123</v>
       </c>
-      <c r="B19" s="0">
-        <v>147</v>
-      </c>
       <c r="C19" s="0">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D19" s="0">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="E19" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F19" s="0">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="G19" s="0">
         <v>0</v>
@@ -1379,27 +1790,45 @@
         <v>0</v>
       </c>
       <c r="U19" s="0">
+        <v>0</v>
+      </c>
+      <c r="V19" s="0">
+        <v>0</v>
+      </c>
+      <c r="W19" s="0">
+        <v>0</v>
+      </c>
+      <c r="X19" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B20" s="0">
-        <v>179</v>
+        <v>116</v>
       </c>
       <c r="C20" s="0">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="D20" s="0">
-        <v>197</v>
+        <v>90</v>
       </c>
       <c r="E20" s="0">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="F20" s="0">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="G20" s="0">
         <v>0</v>
@@ -1444,27 +1873,45 @@
         <v>0</v>
       </c>
       <c r="U20" s="0">
+        <v>0</v>
+      </c>
+      <c r="V20" s="0">
+        <v>0</v>
+      </c>
+      <c r="W20" s="0">
+        <v>0</v>
+      </c>
+      <c r="X20" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B21" s="0">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C21" s="0">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D21" s="0">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="E21" s="0">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="F21" s="0">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="G21" s="0">
         <v>0</v>
@@ -1509,27 +1956,45 @@
         <v>0</v>
       </c>
       <c r="U21" s="0">
+        <v>0</v>
+      </c>
+      <c r="V21" s="0">
+        <v>0</v>
+      </c>
+      <c r="W21" s="0">
+        <v>0</v>
+      </c>
+      <c r="X21" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>198</v>
+        <v>88</v>
       </c>
       <c r="B22" s="0">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="C22" s="0">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="D22" s="0">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="E22" s="0">
-        <v>172</v>
+        <v>41</v>
       </c>
       <c r="F22" s="0">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="G22" s="0">
         <v>0</v>
@@ -1574,27 +2039,45 @@
         <v>0</v>
       </c>
       <c r="U22" s="0">
+        <v>0</v>
+      </c>
+      <c r="V22" s="0">
+        <v>0</v>
+      </c>
+      <c r="W22" s="0">
+        <v>0</v>
+      </c>
+      <c r="X22" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C23" s="0">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="D23" s="0">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="E23" s="0">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="F23" s="0">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="G23" s="0">
         <v>0</v>
@@ -1639,27 +2122,45 @@
         <v>0</v>
       </c>
       <c r="U23" s="0">
+        <v>0</v>
+      </c>
+      <c r="V23" s="0">
+        <v>0</v>
+      </c>
+      <c r="W23" s="0">
+        <v>0</v>
+      </c>
+      <c r="X23" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="B24" s="0">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C24" s="0">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D24" s="0">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E24" s="0">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="F24" s="0">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="G24" s="0">
         <v>0</v>
@@ -1704,27 +2205,45 @@
         <v>0</v>
       </c>
       <c r="U24" s="0">
+        <v>0</v>
+      </c>
+      <c r="V24" s="0">
+        <v>0</v>
+      </c>
+      <c r="W24" s="0">
+        <v>0</v>
+      </c>
+      <c r="X24" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="B25" s="0">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="C25" s="0">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D25" s="0">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="E25" s="0">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="F25" s="0">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="G25" s="0">
         <v>0</v>
@@ -1769,28 +2288,46 @@
         <v>0</v>
       </c>
       <c r="U25" s="0">
+        <v>0</v>
+      </c>
+      <c r="V25" s="0">
+        <v>0</v>
+      </c>
+      <c r="W25" s="0">
+        <v>0</v>
+      </c>
+      <c r="X25" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
+        <v>2</v>
+      </c>
+      <c r="B26" s="0">
+        <v>60</v>
+      </c>
+      <c r="C26" s="0">
+        <v>55</v>
+      </c>
+      <c r="D26" s="0">
+        <v>116</v>
+      </c>
+      <c r="E26" s="0">
+        <v>78</v>
+      </c>
+      <c r="F26" s="0">
         <v>37</v>
       </c>
-      <c r="B26" s="0">
-        <v>18</v>
-      </c>
-      <c r="C26" s="0">
-        <v>62</v>
-      </c>
-      <c r="D26" s="0">
-        <v>46</v>
-      </c>
-      <c r="E26" s="0">
-        <v>179</v>
-      </c>
-      <c r="F26" s="0">
-        <v>183</v>
-      </c>
       <c r="G26" s="0">
         <v>0</v>
       </c>
@@ -1834,6 +2371,24 @@
         <v>0</v>
       </c>
       <c r="U26" s="0">
+        <v>0</v>
+      </c>
+      <c r="V26" s="0">
+        <v>0</v>
+      </c>
+      <c r="W26" s="0">
+        <v>0</v>
+      </c>
+      <c r="X26" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="0">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>